<commit_message>
tuned RF parameters and generated model output. weak performance overall. will consider adding XGBoost models on PCA data later if time allows it. updated metrics XL with RF stats.
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0E25AA-1CDC-4B97-9E8F-55A76B420BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B184D6C-B1D4-4E09-8B82-057736F8FBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="16920" windowHeight="10450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6735" yWindow="0" windowWidth="22170" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Performance Metric</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>R-Squared</t>
+  </si>
+  <si>
+    <t>PCA - XGBoost Model</t>
   </si>
 </sst>
 </file>
@@ -61,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +84,13 @@
       <color theme="1"/>
       <name val="Century"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,10 +119,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -134,9 +145,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -417,18 +432,19 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="50.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.1796875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="46.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -438,7 +454,9 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -446,14 +464,16 @@
       <c r="I1" s="7"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>0.4446</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3">
+        <v>0.45369999999999999</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -464,14 +484,16 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>0.47770000000000001</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3">
+        <v>0.56040000000000001</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -482,14 +504,16 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>0.69120000000000004</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3">
+        <v>0.74860000000000004</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -500,14 +524,16 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>1.7062999999999999</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3">
+        <v>1.5108999999999999</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -518,14 +544,16 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>0.30180000000000001</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3">
+        <v>0.27510000000000001</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -536,14 +564,16 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="9">
+        <v>0.51580000000000004</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>

</xml_diff>

<commit_message>
started fitting OLS models on the non-PCA data. generated performance plots and modified the error XL for each model. moving on to lasso
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B184D6C-B1D4-4E09-8B82-057736F8FBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF050A-3DDB-4F40-BECB-1130BA9F25B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="0" windowWidth="22170" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9045" yWindow="0" windowWidth="19860" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Performance Metric</t>
   </si>
@@ -54,7 +54,13 @@
     <t>R-Squared</t>
   </si>
   <si>
-    <t>PCA - XGBoost Model</t>
+    <t>OLS</t>
+  </si>
+  <si>
+    <t>(1) Market Value (euros)</t>
+  </si>
+  <si>
+    <t>(2) Natural Log of Market Value</t>
   </si>
 </sst>
 </file>
@@ -123,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -139,14 +145,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -429,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -440,62 +455,63 @@
     <col min="1" max="1" width="46.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="34.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="3">
         <v>0.4446</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C3" s="3">
         <v>0.45369999999999999</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.47770000000000001</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.56040000000000001</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="3">
+        <v>6426873.3690999998</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.38640000000000002</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -504,18 +520,22 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>0.69120000000000004</v>
+        <v>0.47770000000000001</v>
       </c>
       <c r="C4" s="3">
-        <v>0.74860000000000004</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+        <v>0.56040000000000001</v>
+      </c>
+      <c r="D4" s="3">
+        <v>106516475775883</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.25890000000000002</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -524,18 +544,22 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>1.7062999999999999</v>
+        <v>0.69120000000000004</v>
       </c>
       <c r="C5" s="3">
-        <v>1.5108999999999999</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+        <v>0.74860000000000004</v>
+      </c>
+      <c r="D5" s="3">
+        <v>10320681.943399999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.50880000000000003</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -544,18 +568,22 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>0.30180000000000001</v>
+        <v>1.7062999999999999</v>
       </c>
       <c r="C6" s="3">
-        <v>0.27510000000000001</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+        <v>1.5108999999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.7145999999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.4899999999999999E-2</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -564,25 +592,56 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.30180000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.27510000000000001</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4481399.3886000002</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.31090000000000001</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B8" s="5">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C8" s="8">
         <v>0.51580000000000004</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="D8" s="8">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.878</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ran untuned lasso models on the standardized data with both versions of the outcome. stored metrics and plots.
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF050A-3DDB-4F40-BECB-1130BA9F25B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAA59C0-3279-4F69-A920-50BD811ECD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9045" yWindow="0" windowWidth="19860" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11190" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Performance Metric</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>(2) Natural Log of Market Value</t>
+  </si>
+  <si>
+    <t>Lasso Regression - Untuned</t>
   </si>
 </sst>
 </file>
@@ -446,35 +449,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="1"/>
+    <col min="6" max="6" width="26.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="12"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -490,13 +497,17 @@
       <c r="E2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -512,15 +523,19 @@
       <c r="E3" s="3">
         <v>0.38640000000000002</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="3">
+        <v>0.3584</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.51549999999999996</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -536,15 +551,19 @@
       <c r="E4" s="3">
         <v>0.25890000000000002</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3">
+        <v>0.41189999999999999</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.42580000000000001</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -560,15 +579,19 @@
       <c r="E5" s="3">
         <v>0.50880000000000003</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="3">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.65259999999999996</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -584,15 +607,19 @@
       <c r="E6" s="3">
         <v>2.4899999999999999E-2</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="3">
+        <v>1.4084000000000001</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.3300000000000003E-2</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -608,15 +635,19 @@
       <c r="E7" s="3">
         <v>0.31090000000000001</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="3">
+        <v>0.25829999999999997</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.4642</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -632,15 +663,20 @@
       <c r="E8" s="8">
         <v>0.878</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="8">
+        <v>0.64410000000000001</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.72419999999999995</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added parameter tuning to the lasso fitting function and removed dummy variables and log mkt val cols. generated visuals and logged errors.
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAA59C0-3279-4F69-A920-50BD811ECD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8D1B1C-38C5-4368-AB83-4D9EA19CE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Performance Metric</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Lasso Regression - Untuned</t>
+  </si>
+  <si>
+    <t>Tuned Lasso Regression</t>
   </si>
 </sst>
 </file>
@@ -449,20 +452,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -503,7 +507,9 @@
       <c r="G2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
     </row>
@@ -529,7 +535,9 @@
       <c r="G3" s="3">
         <v>0.51549999999999996</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="3">
+        <v>0.42770000000000002</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -557,7 +565,9 @@
       <c r="G4" s="3">
         <v>0.42580000000000001</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="3">
+        <v>0.44550000000000001</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -585,7 +595,9 @@
       <c r="G5" s="3">
         <v>0.65259999999999996</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="3">
+        <v>0.66739999999999999</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -613,7 +625,9 @@
       <c r="G6" s="3">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="3">
+        <v>1.6248</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -641,7 +655,9 @@
       <c r="G7" s="3">
         <v>0.4642</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="3">
+        <v>0.29599999999999999</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -669,7 +685,9 @@
       <c r="G8" s="8">
         <v>0.72419999999999995</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="8">
+        <v>0.61509999999999998</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>

</xml_diff>

<commit_message>
added a model performance visualization to the XL
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8D1B1C-38C5-4368-AB83-4D9EA19CE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72DC0B-3B0D-490E-B846-27B250F1281E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,6 +185,1494 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000">
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Model</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0">
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> Performance Metrics by Model Type</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000">
+              <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Absolute Error (MAE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>PCA - OLS Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PCA - Random Forest Model</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(1) Market Value (euros)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tuned Lasso Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$3:$H$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$3:$C$3,Sheet1!$E$3:$H$3)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.4446</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3584</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51549999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42770000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F02-4942-BF06-CA5E834BC2E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Squared Error (MSE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>PCA - OLS Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PCA - Random Forest Model</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(1) Market Value (euros)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tuned Lasso Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$4:$H$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$4:$C$4,Sheet1!$E$4:$H$4)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.47770000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25890000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42580000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44550000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3F02-4942-BF06-CA5E834BC2E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Root Mean Squared Error (RMSE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>PCA - OLS Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PCA - Random Forest Model</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(1) Market Value (euros)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tuned Lasso Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$5:$H$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$5:$C$5,Sheet1!$E$5:$H$5)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.69120000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74860000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64180000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66739999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3F02-4942-BF06-CA5E834BC2E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Absolute Percentage Error (MAPE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>PCA - OLS Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PCA - Random Forest Model</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(1) Market Value (euros)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tuned Lasso Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$6:$H$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$6:$C$6,Sheet1!$E$6:$H$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.7062999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5108999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4084000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3F02-4942-BF06-CA5E834BC2E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median Average Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>PCA - OLS Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PCA - Random Forest Model</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(1) Market Value (euros)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tuned Lasso Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$7:$H$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$7:$C$7,Sheet1!$E$7:$H$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.30180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27510000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31090000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25829999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4642</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29599999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3F02-4942-BF06-CA5E834BC2E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Squared</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>PCA - OLS Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PCA - Random Forest Model</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(1) Market Value (euros)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(2) Natural Log of Market Value</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tuned Lasso Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$8:$H$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$8:$C$8,Sheet1!$E$8:$H$8)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.58499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51580000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.878</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64410000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72419999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61509999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3F02-4942-BF06-CA5E834BC2E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1394231248"/>
+        <c:axId val="1394239888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1394231248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1394239888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1394239888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1394231248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1186132</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>120050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1725282</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>143774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{262DCAF2-1937-C3F6-65BF-A6254C1A680B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -697,5 +2185,6 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-ran the random forest model with tuned parameters. stored metrics and plots. FE model next
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72DC0B-3B0D-490E-B846-27B250F1281E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F094E2-47D3-45CB-A073-65BC30C87A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1875" yWindow="1650" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Performance Metric</t>
   </si>
@@ -68,6 +68,9 @@
   <si>
     <t>Tuned Lasso Regression</t>
   </si>
+  <si>
+    <t>Tuned Random Forest</t>
+  </si>
 </sst>
 </file>
 
@@ -76,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +88,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Century"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Century"/>
@@ -133,9 +129,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -149,9 +145,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -327,7 +320,7 @@
                   <c:v>(2) Natural Log of Market Value</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Tuned Lasso Regression</c:v>
+                  <c:v>(1) Market Value (euros)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -427,7 +420,7 @@
                   <c:v>(2) Natural Log of Market Value</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Tuned Lasso Regression</c:v>
+                  <c:v>(1) Market Value (euros)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -527,7 +520,7 @@
                   <c:v>(2) Natural Log of Market Value</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Tuned Lasso Regression</c:v>
+                  <c:v>(1) Market Value (euros)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -629,7 +622,7 @@
                   <c:v>(2) Natural Log of Market Value</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Tuned Lasso Regression</c:v>
+                  <c:v>(1) Market Value (euros)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -731,7 +724,7 @@
                   <c:v>(2) Natural Log of Market Value</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Tuned Lasso Regression</c:v>
+                  <c:v>(1) Market Value (euros)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -833,7 +826,7 @@
                   <c:v>(2) Natural Log of Market Value</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Tuned Lasso Regression</c:v>
+                  <c:v>(1) Market Value (euros)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1639,15 +1632,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1186132</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>120050</xdr:rowOff>
+      <xdr:colOff>1311934</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1725282</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>143774</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>125801</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>35943</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1940,68 +1933,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="46.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2026,12 +2024,14 @@
       <c r="H3" s="3">
         <v>0.42770000000000002</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="3">
+        <v>5966124.7529999996</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2056,12 +2056,14 @@
       <c r="H4" s="3">
         <v>0.44550000000000001</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="3">
+        <v>105522343876105</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2086,12 +2088,14 @@
       <c r="H5" s="3">
         <v>0.66739999999999999</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="3">
+        <v>10272406.917400001</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2116,12 +2120,14 @@
       <c r="H6" s="3">
         <v>1.6248</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="3">
+        <v>0.88060000000000005</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -2146,37 +2152,41 @@
       <c r="H7" s="3">
         <v>0.29599999999999999</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="3">
+        <v>3039250</v>
+      </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="37" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>0.51580000000000004</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0.81899999999999995</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>0.878</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>0.64410000000000001</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>0.72419999999999995</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>0.61509999999999998</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="7">
+        <v>0.76039999999999996</v>
+      </c>
       <c r="J8" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran OLS models on only features from RF model. also stored outputs and made some XL visuals for deck.
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F094E2-47D3-45CB-A073-65BC30C87A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87FF0EA-5455-4268-9247-40304A07AF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1650" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>Performance Metric</t>
   </si>
@@ -71,6 +72,27 @@
   <si>
     <t>Tuned Random Forest</t>
   </si>
+  <si>
+    <t>Target Variable: Standardized Market Value</t>
+  </si>
+  <si>
+    <t>Untuned Lasso Regression</t>
+  </si>
+  <si>
+    <t>Target Variable: Natural Log of Market Value</t>
+  </si>
+  <si>
+    <t>Naïve OLS</t>
+  </si>
+  <si>
+    <t>Target Variable: Market Value (euros)</t>
+  </si>
+  <si>
+    <t>OLS with Random Forest Features Only</t>
+  </si>
+  <si>
+    <t>OLS with Random Forest Features</t>
+  </si>
 </sst>
 </file>
 
@@ -101,15 +123,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -126,12 +154,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -162,6 +276,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,10 +359,897 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="103"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Performance Metrics by Model Type</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Absolute Error (MAE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PCA - OLS Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>PCA - Random Forest Model</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Tuned Lasso Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Standardized Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.4446</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3584</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42770000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E06-44A9-95A5-618EF7837405}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Squared Error (MSE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PCA - OLS Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>PCA - Random Forest Model</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Tuned Lasso Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Standardized Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.47770000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44550000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E06-44A9-95A5-618EF7837405}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Root Mean Squared Error (RMSE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg2"/>
+                    </a:solidFill>
+                    <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PCA - OLS Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>PCA - Random Forest Model</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Tuned Lasso Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Standardized Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.69120000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74860000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64180000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66739999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0E06-44A9-95A5-618EF7837405}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Absolute Percentage Error (MAPE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PCA - OLS Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>PCA - Random Forest Model</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Tuned Lasso Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Standardized Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.7062999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5108999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4084000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0E06-44A9-95A5-618EF7837405}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median Average Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PCA - OLS Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>PCA - Random Forest Model</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Tuned Lasso Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Standardized Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.30180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27510000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25829999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29599999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0E06-44A9-95A5-618EF7837405}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Squared</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PCA - OLS Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>PCA - Random Forest Model</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Tuned Lasso Regression</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Standardized Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.58499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51580000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64410000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61509999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0E06-44A9-95A5-618EF7837405}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="445366079"/>
+        <c:axId val="445366559"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="445366079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445366559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="445366559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445366079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -214,20 +1273,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000">
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
                 <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>Model</a:t>
+              <a:t>Performance Metrics by Model Type</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="2000" baseline="0">
-                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
-              </a:rPr>
-              <a:t> Performance Metrics by Model Type</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="2000">
-              <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -263,15 +1319,16 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet2!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -281,88 +1338,82 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>PCA - OLS Regression</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PCA - Random Forest Model</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Naïve OLS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Tuned Random Forest</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>OLS with Random Forest Features</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Natural Log of Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$3:$H$3</c15:sqref>
+                    <c15:sqref>Sheet2!$B$4:$I$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$3:$C$3,Sheet1!$E$3:$H$3)</c:f>
+              <c:f>Sheet2!$F$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.4446</c:v>
+                  <c:v>0.43490000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45369999999999999</c:v>
+                  <c:v>0.51549999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38640000000000002</c:v>
+                  <c:v>0.47970000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3584</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.51549999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.42770000000000002</c:v>
+                  <c:v>1.1878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3F02-4942-BF06-CA5E834BC2E7}"/>
+              <c16:uniqueId val="{00000000-F289-49C1-81F7-319F9BDD04F7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -371,7 +1422,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet2!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -381,88 +1432,82 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>PCA - OLS Regression</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PCA - Random Forest Model</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Naïve OLS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Tuned Random Forest</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>OLS with Random Forest Features</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Natural Log of Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$4:$H$4</c15:sqref>
+                    <c15:sqref>Sheet2!$B$5:$I$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$4:$C$4,Sheet1!$E$4:$H$4)</c:f>
+              <c:f>Sheet2!$F$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.47770000000000001</c:v>
+                  <c:v>0.32329999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56040000000000001</c:v>
+                  <c:v>0.42580000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25890000000000002</c:v>
+                  <c:v>0.3861</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41189999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.42580000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.44550000000000001</c:v>
+                  <c:v>2.2372999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3F02-4942-BF06-CA5E834BC2E7}"/>
+              <c16:uniqueId val="{00000001-F289-49C1-81F7-319F9BDD04F7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -471,7 +1516,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet2!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -481,88 +1526,140 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>PCA - OLS Regression</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PCA - Random Forest Model</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Naïve OLS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Tuned Random Forest</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>OLS with Random Forest Features</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Natural Log of Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$5:$H$5</c15:sqref>
+                    <c15:sqref>Sheet2!$B$6:$I$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$5:$C$5,Sheet1!$E$5:$H$5)</c:f>
+              <c:f>Sheet2!$F$6:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.69120000000000004</c:v>
+                  <c:v>0.56859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74860000000000004</c:v>
+                  <c:v>0.65259999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50880000000000003</c:v>
+                  <c:v>0.62139999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64180000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.65259999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.66739999999999999</c:v>
+                  <c:v>1.4958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3F02-4942-BF06-CA5E834BC2E7}"/>
+              <c16:uniqueId val="{00000002-F289-49C1-81F7-319F9BDD04F7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -571,7 +1668,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>Sheet2!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -581,90 +1678,82 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>PCA - OLS Regression</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PCA - Random Forest Model</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Naïve OLS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Tuned Random Forest</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>OLS with Random Forest Features</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Natural Log of Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$6:$H$6</c15:sqref>
+                    <c15:sqref>Sheet2!$B$7:$I$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$6:$C$6,Sheet1!$E$6:$H$6)</c:f>
+              <c:f>Sheet2!$F$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.7062999999999999</c:v>
+                  <c:v>2.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5108999999999999</c:v>
+                  <c:v>3.3300000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4899999999999999E-2</c:v>
+                  <c:v>3.09E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4084000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.3300000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6248</c:v>
+                  <c:v>7.6100000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3F02-4942-BF06-CA5E834BC2E7}"/>
+              <c16:uniqueId val="{00000003-F289-49C1-81F7-319F9BDD04F7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -673,7 +1762,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet2!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -683,90 +1772,82 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>PCA - OLS Regression</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PCA - Random Forest Model</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Naïve OLS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Tuned Random Forest</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>OLS with Random Forest Features</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Natural Log of Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$7:$H$7</c15:sqref>
+                    <c15:sqref>Sheet2!$B$8:$I$8</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$7:$C$7,Sheet1!$E$7:$H$7)</c:f>
+              <c:f>Sheet2!$F$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.30180000000000001</c:v>
+                  <c:v>0.35039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27510000000000001</c:v>
+                  <c:v>0.4642</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31090000000000001</c:v>
+                  <c:v>0.40200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25829999999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.4642</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.29599999999999999</c:v>
+                  <c:v>0.9798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-3F02-4942-BF06-CA5E834BC2E7}"/>
+              <c16:uniqueId val="{00000004-F289-49C1-81F7-319F9BDD04F7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -775,7 +1856,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet2!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -785,90 +1866,140 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$H$2</c15:sqref>
+                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$2:$C$2,Sheet1!$E$2:$H$2)</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>PCA - OLS Regression</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PCA - Random Forest Model</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(2) Natural Log of Market Value</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(1) Market Value (euros)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Naïve OLS</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Untuned Lasso Regression</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Tuned Random Forest</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>OLS with Random Forest Features</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Target Variable: Natural Log of Market Value</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$8:$H$8</c15:sqref>
+                    <c15:sqref>Sheet2!$B$9:$I$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$B$8:$C$8,Sheet1!$E$8:$H$8)</c:f>
+              <c:f>Sheet2!$F$9:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.58499999999999996</c:v>
+                  <c:v>0.82299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51580000000000004</c:v>
+                  <c:v>0.72419999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.878</c:v>
+                  <c:v>0.74990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64410000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.72419999999999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.61509999999999998</c:v>
+                  <c:v>0.99099999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-3F02-4942-BF06-CA5E834BC2E7}"/>
+              <c16:uniqueId val="{00000005-F289-49C1-81F7-319F9BDD04F7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -880,12 +2011,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1394231248"/>
-        <c:axId val="1394239888"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1648392656"/>
+        <c:axId val="1648393136"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="1394231248"/>
+        <c:axId val="1648392656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,15 +2044,15 @@
           <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:pPr algn="ctr">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Century" panose="02040604050505020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -928,7 +2060,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1394239888"/>
+        <c:crossAx val="1648393136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -936,7 +2068,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1394239888"/>
+        <c:axId val="1648393136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,8 +2103,8 @@
           <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:pPr algn="ctr">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -987,7 +2119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1394231248"/>
+        <c:crossAx val="1648392656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1000,7 +2132,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1014,7 +2146,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1075,44 +2207,19 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
-  <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1220,11 +2327,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1235,11 +2337,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1271,9 +2368,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1329,22 +2423,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1449,8 +2544,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1582,19 +2677,525 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1632,22 +3233,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1311934</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>12219</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>125801</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>35943</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1038226</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{262DCAF2-1937-C3F6-65BF-A6254C1A680B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AC4F477-1244-A43E-27FC-186550C211CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1660,6 +3261,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1443037</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5AB83FD-91FC-9107-4A8A-68F7971632C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1931,27 +3568,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="G8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="51.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="1"/>
+    <col min="10" max="10" width="40.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1966,10 +3604,12 @@
       <c r="H1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="I1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1995,11 +3635,13 @@
         <v>10</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2027,11 +3669,13 @@
       <c r="I3" s="3">
         <v>5966124.7529999996</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="3">
+        <v>0.47970000000000002</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2059,11 +3703,13 @@
       <c r="I4" s="3">
         <v>105522343876105</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3">
+        <v>0.3861</v>
+      </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2091,11 +3737,13 @@
       <c r="I5" s="3">
         <v>10272406.917400001</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="3">
+        <v>0.62139999999999995</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2123,11 +3771,13 @@
       <c r="I6" s="3">
         <v>0.88060000000000005</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="3">
+        <v>3.09E-2</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -2155,11 +3805,13 @@
       <c r="I7" s="3">
         <v>3039250</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="3">
+        <v>0.40200000000000002</v>
+      </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2187,12 +3839,616 @@
       <c r="I8" s="7">
         <v>0.76039999999999996</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="7">
+        <v>0.74990000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="23"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+    </row>
+    <row r="13" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="17">
+        <v>0.4446</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0.45369999999999999</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0.3584</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0.42770000000000002</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.43490000000000001</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0.47970000000000002</v>
+      </c>
+      <c r="I14" s="19">
+        <v>7411171.3448999999</v>
+      </c>
+      <c r="J14" s="18">
+        <v>5966124.7529999996</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="17">
+        <v>0.47770000000000001</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.56040000000000001</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.41189999999999999</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.32329999999999998</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0.42580000000000001</v>
+      </c>
+      <c r="H15" s="18">
+        <v>0.3861</v>
+      </c>
+      <c r="I15" s="17">
+        <v>134185071187122</v>
+      </c>
+      <c r="J15" s="18">
+        <v>105522343876105</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="17">
+        <v>0.69120000000000004</v>
+      </c>
+      <c r="C16" s="18">
+        <v>0.74860000000000004</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="E16" s="22">
+        <v>0.66739999999999999</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.56859999999999999</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0.65259999999999996</v>
+      </c>
+      <c r="H16" s="18">
+        <v>0.62139999999999995</v>
+      </c>
+      <c r="I16" s="17">
+        <v>11583828.0023</v>
+      </c>
+      <c r="J16" s="18">
+        <v>10272406.917400001</v>
+      </c>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+    </row>
+    <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="17">
+        <v>1.7062999999999999</v>
+      </c>
+      <c r="C17" s="18">
+        <v>1.5108999999999999</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1.4084000000000001</v>
+      </c>
+      <c r="E17" s="22">
+        <v>1.6248</v>
+      </c>
+      <c r="F17" s="17">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G17" s="18">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="H17" s="18">
+        <v>3.09E-2</v>
+      </c>
+      <c r="I17" s="17">
+        <v>1.5906</v>
+      </c>
+      <c r="J17" s="18">
+        <v>0.88060000000000005</v>
+      </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="17">
+        <v>0.30180000000000001</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0.27510000000000001</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.25829999999999997</v>
+      </c>
+      <c r="E18" s="22">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.35039999999999999</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0.4642</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="I18" s="17">
+        <v>5113693.9995999997</v>
+      </c>
+      <c r="J18" s="18">
+        <v>3039250</v>
+      </c>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+    </row>
+    <row r="19" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="26">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="C19" s="27">
+        <v>0.51580000000000004</v>
+      </c>
+      <c r="D19" s="27">
+        <v>0.64410000000000001</v>
+      </c>
+      <c r="E19" s="28">
+        <v>0.61509999999999998</v>
+      </c>
+      <c r="F19" s="29">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G19" s="27">
+        <v>0.72419999999999995</v>
+      </c>
+      <c r="H19" s="27">
+        <v>0.74990000000000001</v>
+      </c>
+      <c r="I19" s="29">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="J19" s="27">
+        <v>0.76039999999999996</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25FB9659-1A99-4885-BF7B-C729BCF2C6D6}">
+  <dimension ref="A2:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+    </row>
+    <row r="3" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0.4446</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.45369999999999999</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.3584</v>
+      </c>
+      <c r="E4" s="22">
+        <v>0.42770000000000002</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.43490000000000001</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0.47970000000000002</v>
+      </c>
+      <c r="I4" s="18">
+        <v>1.1878</v>
+      </c>
+      <c r="J4" s="19">
+        <v>7411171.3448999999</v>
+      </c>
+      <c r="K4" s="18">
+        <v>5966124.7529999996</v>
+      </c>
+      <c r="L4" s="18">
+        <v>7630631.9583000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17">
+        <v>0.47770000000000001</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.56040000000000001</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.41189999999999999</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.32329999999999998</v>
+      </c>
+      <c r="G5" s="18">
+        <v>0.42580000000000001</v>
+      </c>
+      <c r="H5" s="18">
+        <v>0.3861</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2.2372999999999998</v>
+      </c>
+      <c r="J5" s="17">
+        <v>134185071187122</v>
+      </c>
+      <c r="K5" s="18">
+        <v>105522343876105</v>
+      </c>
+      <c r="L5" s="18">
+        <v>165363072391684</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0.69120000000000004</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.74860000000000004</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.66739999999999999</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.56859999999999999</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.65259999999999996</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.62139999999999995</v>
+      </c>
+      <c r="I6" s="18">
+        <v>1.4958</v>
+      </c>
+      <c r="J6" s="17">
+        <v>11583828.0023</v>
+      </c>
+      <c r="K6" s="18">
+        <v>10272406.917400001</v>
+      </c>
+      <c r="L6" s="18">
+        <v>12859357.386399999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1.7062999999999999</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1.5108999999999999</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1.4084000000000001</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1.6248</v>
+      </c>
+      <c r="F7" s="17">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>3.09E-2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="J7" s="17">
+        <v>1.5906</v>
+      </c>
+      <c r="K7" s="18">
+        <v>0.88060000000000005</v>
+      </c>
+      <c r="L7" s="18">
+        <v>1.4092</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0.30180000000000001</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.27510000000000001</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.25829999999999997</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.35039999999999999</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.4642</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0.9798</v>
+      </c>
+      <c r="J8" s="17">
+        <v>5113693.9995999997</v>
+      </c>
+      <c r="K8" s="18">
+        <v>3039250</v>
+      </c>
+      <c r="L8" s="18">
+        <v>4436475.5537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="26">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="C9" s="27">
+        <v>0.51580000000000004</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0.64410000000000001</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0.61509999999999998</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0.72419999999999995</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0.74990000000000001</v>
+      </c>
+      <c r="I9" s="27">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="J9" s="29">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="K9" s="27">
+        <v>0.76039999999999996</v>
+      </c>
+      <c r="L9" s="27">
+        <v>0.78300000000000003</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
ran position-specific OLS models. stored outputs.
</commit_message>
<xml_diff>
--- a/analysis-results/Model Performance Metrics.xlsx
+++ b/analysis-results/Model Performance Metrics.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmart\Documents\GitHub\player-valuation-model\analysis-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87FF0EA-5455-4268-9247-40304A07AF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5571F92A-CF76-481A-9DCB-B3901D80DC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Main" sheetId="2" r:id="rId2"/>
+    <sheet name="Position Models" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
   <si>
     <t>Performance Metric</t>
   </si>
@@ -93,6 +94,15 @@
   <si>
     <t>OLS with Random Forest Features</t>
   </si>
+  <si>
+    <t>OLS - Defenders Only</t>
+  </si>
+  <si>
+    <t>OLS - Forwards Only</t>
+  </si>
+  <si>
+    <t>OLS - Midfielders Only</t>
+  </si>
 </sst>
 </file>
 
@@ -137,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -240,12 +250,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -273,12 +305,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,13 +318,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -308,9 +328,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -328,12 +345,44 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +484,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$4</c:f>
+              <c:f>Main!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -461,7 +510,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:f>Main!$B$2:$E$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -488,7 +537,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$4:$E$4</c:f>
+              <c:f>Main!$B$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -518,7 +567,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$5</c:f>
+              <c:f>Main!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -544,7 +593,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:f>Main!$B$2:$E$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -571,7 +620,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$5:$E$5</c:f>
+              <c:f>Main!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -601,7 +650,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$6</c:f>
+              <c:f>Main!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -679,7 +728,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:f>Main!$B$2:$E$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -706,7 +755,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$6:$E$6</c:f>
+              <c:f>Main!$B$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -736,7 +785,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$7</c:f>
+              <c:f>Main!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -762,7 +811,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:f>Main!$B$2:$E$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -789,7 +838,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$7:$E$7</c:f>
+              <c:f>Main!$B$7:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -819,7 +868,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$8</c:f>
+              <c:f>Main!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -845,7 +894,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:f>Main!$B$2:$E$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -872,7 +921,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$8:$E$8</c:f>
+              <c:f>Main!$B$8:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -902,7 +951,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$9</c:f>
+              <c:f>Main!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -983,7 +1032,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$2:$E$3</c:f>
+              <c:f>Main!$B$2:$E$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1010,7 +1059,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$9:$E$9</c:f>
+              <c:f>Main!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1328,7 +1377,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$4</c:f>
+              <c:f>Main!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1354,11 +1403,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
+                    <c15:sqref>Main!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:f>Main!$F$2:$I$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1388,11 +1437,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$4:$I$4</c15:sqref>
+                    <c15:sqref>Main!$B$4:$I$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$4:$I$4</c:f>
+              <c:f>Main!$F$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1422,7 +1471,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$5</c:f>
+              <c:f>Main!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1448,11 +1497,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
+                    <c15:sqref>Main!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:f>Main!$F$2:$I$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1482,11 +1531,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$5:$I$5</c15:sqref>
+                    <c15:sqref>Main!$B$5:$I$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$5:$I$5</c:f>
+              <c:f>Main!$F$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1516,7 +1565,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$6</c:f>
+              <c:f>Main!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1600,11 +1649,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
+                    <c15:sqref>Main!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:f>Main!$F$2:$I$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1634,11 +1683,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$6:$I$6</c15:sqref>
+                    <c15:sqref>Main!$B$6:$I$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$6:$I$6</c:f>
+              <c:f>Main!$F$6:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1668,7 +1717,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$7</c:f>
+              <c:f>Main!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1694,11 +1743,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
+                    <c15:sqref>Main!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:f>Main!$F$2:$I$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1728,11 +1777,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$7:$I$7</c15:sqref>
+                    <c15:sqref>Main!$B$7:$I$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$7:$I$7</c:f>
+              <c:f>Main!$F$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1762,7 +1811,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$8</c:f>
+              <c:f>Main!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1788,11 +1837,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
+                    <c15:sqref>Main!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:f>Main!$F$2:$I$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1822,11 +1871,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$8:$I$8</c15:sqref>
+                    <c15:sqref>Main!$B$8:$I$8</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$8:$I$8</c:f>
+              <c:f>Main!$F$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1856,7 +1905,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$9</c:f>
+              <c:f>Main!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1940,11 +1989,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$2:$I$3</c15:sqref>
+                    <c15:sqref>Main!$B$2:$I$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$2:$I$3</c:f>
+              <c:f>Main!$F$2:$I$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1974,11 +2023,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet2!$B$9:$I$9</c15:sqref>
+                    <c15:sqref>Main!$B$9:$I$9</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet2!$F$9:$I$9</c:f>
+              <c:f>Main!$F$9:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2206,6 +2255,650 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Position Models'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Absolute Error (MAE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Position Models'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>OLS - Defenders Only</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OLS - Midfielders Only</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OLS - Forwards Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Position Models'!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.45710000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44690000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43969999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B16-4BF8-8326-8DD8E9255BF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Position Models'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Squared Error (MSE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Position Models'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>OLS - Defenders Only</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OLS - Midfielders Only</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OLS - Forwards Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Position Models'!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.40310000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32569999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0B16-4BF8-8326-8DD8E9255BF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Position Models'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Root Mean Squared Error (RMSE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Position Models'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>OLS - Defenders Only</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OLS - Midfielders Only</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OLS - Forwards Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Position Models'!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.63490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56720000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57069999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0B16-4BF8-8326-8DD8E9255BF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Position Models'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Absolute Percentage Error (MAPE)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Position Models'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>OLS - Defenders Only</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OLS - Midfielders Only</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OLS - Forwards Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Position Models'!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.87E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8299999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0B16-4BF8-8326-8DD8E9255BF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Position Models'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median Average Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Position Models'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>OLS - Defenders Only</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OLS - Midfielders Only</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OLS - Forwards Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Position Models'!$B$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.36380000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37369999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35220000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0B16-4BF8-8326-8DD8E9255BF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Position Models'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Squared</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Position Models'!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>OLS - Defenders Only</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OLS - Midfielders Only</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OLS - Forwards Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Position Models'!$B$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.80100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82899999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84199999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0B16-4BF8-8326-8DD8E9255BF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="65700959"/>
+        <c:axId val="65689439"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="65700959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65689439"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65689439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65700959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
   <a:schemeClr val="accent1"/>
@@ -2215,6 +2908,46 @@
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
   <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -2724,6 +3457,511 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3297,6 +4535,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1419225</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2904C0BB-1D38-4152-C4D6-4221661D6664}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3593,21 +4872,21 @@
       <c r="A1" s="10"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="12"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -3844,278 +5123,278 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24" t="s">
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="15">
         <v>0.4446</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="14">
         <v>0.45369999999999999</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="14">
         <v>0.3584</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="18">
         <v>0.42770000000000002</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="15">
         <v>0.43490000000000001</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="14">
         <v>0.51549999999999996</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="14">
         <v>0.47970000000000002</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="16">
         <v>7411171.3448999999</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="14">
         <v>5966124.7529999996</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="15">
         <v>0.47770000000000001</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="14">
         <v>0.56040000000000001</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="14">
         <v>0.41189999999999999</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="18">
         <v>0.44550000000000001</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="15">
         <v>0.32329999999999998</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="14">
         <v>0.42580000000000001</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="14">
         <v>0.3861</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="15">
         <v>134185071187122</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="14">
         <v>105522343876105</v>
       </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="15">
         <v>0.69120000000000004</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="14">
         <v>0.74860000000000004</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="14">
         <v>0.64180000000000004</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="18">
         <v>0.66739999999999999</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="15">
         <v>0.56859999999999999</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="14">
         <v>0.65259999999999996</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="14">
         <v>0.62139999999999995</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="15">
         <v>11583828.0023</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="14">
         <v>10272406.917400001</v>
       </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="15">
         <v>1.7062999999999999</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="14">
         <v>1.5108999999999999</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="14">
         <v>1.4084000000000001</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="18">
         <v>1.6248</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="15">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="14">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="14">
         <v>3.09E-2</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="15">
         <v>1.5906</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="14">
         <v>0.88060000000000005</v>
       </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="15">
         <v>0.30180000000000001</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="14">
         <v>0.27510000000000001</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="14">
         <v>0.25829999999999997</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="18">
         <v>0.29599999999999999</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="15">
         <v>0.35039999999999999</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="14">
         <v>0.4642</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="14">
         <v>0.40200000000000002</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="15">
         <v>5113693.9995999997</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="14">
         <v>3039250</v>
       </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="21">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="22">
         <v>0.51580000000000004</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="22">
         <v>0.64410000000000001</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="23">
         <v>0.61509999999999998</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="24">
         <v>0.82299999999999995</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="22">
         <v>0.72419999999999995</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H19" s="22">
         <v>0.74990000000000001</v>
       </c>
-      <c r="I19" s="29">
+      <c r="I19" s="24">
         <v>0.73899999999999999</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J19" s="22">
         <v>0.76039999999999996</v>
       </c>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4137,7 +5416,7 @@
   <dimension ref="A2:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4157,289 +5436,289 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="24" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <v>0.4446</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="14">
         <v>0.45369999999999999</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="14">
         <v>0.3584</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="18">
         <v>0.42770000000000002</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="15">
         <v>0.43490000000000001</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="14">
         <v>0.51549999999999996</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>0.47970000000000002</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>1.1878</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="16">
         <v>7411171.3448999999</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="14">
         <v>5966124.7529999996</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="14">
         <v>7630631.9583000001</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>0.47770000000000001</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <v>0.56040000000000001</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="14">
         <v>0.41189999999999999</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="18">
         <v>0.44550000000000001</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="15">
         <v>0.32329999999999998</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <v>0.42580000000000001</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="14">
         <v>0.3861</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="14">
         <v>2.2372999999999998</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="15">
         <v>134185071187122</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>105522343876105</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="14">
         <v>165363072391684</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>0.69120000000000004</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>0.74860000000000004</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="14">
         <v>0.64180000000000004</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="18">
         <v>0.66739999999999999</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="15">
         <v>0.56859999999999999</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="14">
         <v>0.65259999999999996</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>0.62139999999999995</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>1.4958</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="15">
         <v>11583828.0023</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>10272406.917400001</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>12859357.386399999</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="15">
         <v>1.7062999999999999</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="14">
         <v>1.5108999999999999</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="14">
         <v>1.4084000000000001</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="18">
         <v>1.6248</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="15">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="14">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>3.09E-2</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>7.6100000000000001E-2</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="15">
         <v>1.5906</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="14">
         <v>0.88060000000000005</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="14">
         <v>1.4092</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="15">
         <v>0.30180000000000001</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>0.27510000000000001</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>0.25829999999999997</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="18">
         <v>0.29599999999999999</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="15">
         <v>0.35039999999999999</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>0.4642</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>0.40200000000000002</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>0.9798</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="15">
         <v>5113693.9995999997</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="14">
         <v>3039250</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>4436475.5537</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="21">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="22">
         <v>0.51580000000000004</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="22">
         <v>0.64410000000000001</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="23">
         <v>0.61509999999999998</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="24">
         <v>0.82299999999999995</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="22">
         <v>0.72419999999999995</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="22">
         <v>0.74990000000000001</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="22">
         <v>0.99099999999999999</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="24">
         <v>0.73899999999999999</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="22">
         <v>0.76039999999999996</v>
       </c>
-      <c r="L9" s="27">
+      <c r="L9" s="22">
         <v>0.78300000000000003</v>
       </c>
     </row>
@@ -4453,4 +5732,667 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50062246-7F56-4382-9920-F46FF06D738C}">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+    </row>
+    <row r="3" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+    </row>
+    <row r="4" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.45710000000000001</v>
+      </c>
+      <c r="C4" s="37">
+        <v>0.44690000000000002</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0.43969999999999998</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+    </row>
+    <row r="5" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.40310000000000001</v>
+      </c>
+      <c r="C5" s="35">
+        <v>0.32169999999999999</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.32569999999999999</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+    </row>
+    <row r="6" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.63490000000000002</v>
+      </c>
+      <c r="C6" s="35">
+        <v>0.56720000000000004</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.57069999999999999</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+    </row>
+    <row r="7" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="C7" s="35">
+        <v>2.87E-2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2.8299999999999999E-2</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+    </row>
+    <row r="8" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0.36380000000000001</v>
+      </c>
+      <c r="C8" s="35">
+        <v>0.37369999999999998</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.35220000000000001</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+    </row>
+    <row r="9" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="21">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="C9" s="36">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="D9" s="34">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>